<commit_message>
add mapped ontology terms
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/apidb/ApiCommonData/trunk@70752 735e2a04-f8fc-0310-8a1b-f2942603c481
</commit_message>
<xml_diff>
--- a/Load/src/ontology/ICEMR/ICEMR protein array/NTR/20151112_ICEMR_array.xlsx
+++ b/Load/src/ontology/ICEMR/ICEMR protein array/NTR/20151112_ICEMR_array.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="23760" windowHeight="9960"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="25230" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="term mappings" sheetId="5" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="new terms" sheetId="1" r:id="rId3"/>
     <sheet name="new import terms" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="234">
   <si>
     <t>Characteristics[age]</t>
   </si>
@@ -628,7 +628,127 @@
     <t>Ontology Term Label</t>
   </si>
   <si>
-    <t>halogroup</t>
+    <t>http://purl.obolibrary.org/obo/DOID_9065 #leishmaniasis</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DOID_9111 #cutaneous Leishmaniasis</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DOID_9146 #visceral leishmaniasis</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DOID_9181 #amoebiasis</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IDO_0000566 #primary infection</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/IDO_0000586 #infection</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000181 #population</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0000852 #record of missing knowledge</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0001554 #rate measurement datum</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OGMS_0000027 #clinical phenotype</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000036 #year</t>
+  </si>
+  <si>
+    <t>half life datum (t 1/2)</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000275</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000276</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000277</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000278</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000279</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000280</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000281</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000282</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000283</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000284</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000285</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000286</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000287</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000288</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000289</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000290</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000291</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000292</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000293</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000294</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000295</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000296</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000297</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000298</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000299</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/EUPATH_0000300</t>
+  </si>
+  <si>
+    <t>Omar: "no idea what these mean and agree that having them as is useless", so not add ontology term</t>
+  </si>
+  <si>
+    <t>will contact submitters for acronyms of treatment outcome, then relabel the ontology terms</t>
+  </si>
+  <si>
+    <t>Comments</t>
   </si>
 </sst>
 </file>
@@ -783,7 +903,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -815,6 +935,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1118,10 +1239,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1129,10 +1250,11 @@
     <col min="1" max="1" width="57.28515625" customWidth="1"/>
     <col min="2" max="2" width="42.85546875" style="10" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="9" t="s">
         <v>75</v>
       </c>
@@ -1142,8 +1264,11 @@
       <c r="D1" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1157,76 +1282,88 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D4" t="s">
+      <c r="C4" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="D4" s="25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C6" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="D6" s="25" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D8" t="s">
+      <c r="C8" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8" s="25" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D10" s="25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1240,47 +1377,59 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D13" s="25" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="C15" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="D16" s="25" t="s">
         <v>120</v>
       </c>
     </row>
@@ -1291,7 +1440,10 @@
       <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="D17" s="25" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1302,7 +1454,10 @@
       <c r="B18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="D18" s="25" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1313,7 +1468,10 @@
       <c r="B19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D19" s="25" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1324,7 +1482,10 @@
       <c r="B20" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="D20" s="25" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1335,7 +1496,10 @@
       <c r="B21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21" s="25" t="s">
         <v>129</v>
       </c>
     </row>
@@ -1430,7 +1594,10 @@
       <c r="B28" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" s="25" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1441,8 +1608,11 @@
       <c r="B29" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="D29" t="s">
-        <v>193</v>
+      <c r="C29" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1478,152 +1648,191 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>28</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C33" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D33" s="25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E35" s="23" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="24"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
       <c r="B37" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D37" t="s">
+      <c r="C37" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D37" s="25" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="C39" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
       <c r="B40" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="D40" s="25" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D41" t="s">
+      <c r="C41" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="D41" s="25" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C42" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="D42" s="25" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
       <c r="B43" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D43" t="s">
+      <c r="C43" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="D43" s="25" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
       <c r="B44" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="C44" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="D44" s="25" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D45" s="11" t="s">
+      <c r="C45" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="D45" s="25" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
       <c r="B46" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D46" s="11" t="s">
+      <c r="C46" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="D46" s="25" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
       <c r="B47" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="C47" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="D47" s="25" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -1670,8 +1879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2270,7 @@
       <c r="B25" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D25" t="s">
@@ -2487,6 +2696,7 @@
     <hyperlink ref="A57" r:id="rId3"/>
     <hyperlink ref="A58" r:id="rId4"/>
     <hyperlink ref="A60" r:id="rId5"/>
+    <hyperlink ref="C25" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2503,7 +2713,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2899,10 +3109,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,10 +3125,10 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>152</v>
@@ -2929,55 +3139,55 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>164</v>
+        <v>168</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>64</v>
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>162</v>
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" t="s">
-        <v>169</v>
+        <v>112</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>171</v>
       </c>
       <c r="D5" t="s">
         <v>170</v>
@@ -2985,55 +3195,55 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="B6" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="C6" t="s">
-        <v>168</v>
+        <v>95</v>
       </c>
       <c r="D6" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
       <c r="B8" t="s">
-        <v>112</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>171</v>
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>178</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>177</v>
-      </c>
-      <c r="B9" t="s">
-        <v>87</v>
+        <v>161</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>162</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="D9" t="s">
         <v>156</v>
@@ -3041,30 +3251,30 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" t="s">
-        <v>92</v>
+        <v>154</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>164</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>155</v>
       </c>
       <c r="D10" t="s">
-        <v>179</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
+        <v>80</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="C11" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3081,14 +3291,113 @@
         <v>181</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D13" t="s">
+        <v>156</v>
+      </c>
+    </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B16" t="s">
+        <v>169</v>
+      </c>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>202</v>
+      </c>
+      <c r="B25" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="A12" r:id="rId1" display="http://www.ontobee.org/ontology/UO?iri=http://purl.obolibrary.org/obo/UO_0000036"/>
   </hyperlinks>

</xml_diff>